<commit_message>
Quan ly giao dien
</commit_message>
<xml_diff>
--- a/DuLieuNhipTim/2025-12/2025-12-16.xlsx
+++ b/DuLieuNhipTim/2025-12/2025-12-16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -902,6 +902,1146 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>10:33:09</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1765855989.320874</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>46</v>
+      </c>
+      <c r="E18" t="n">
+        <v>80</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>10:33:29</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1765856009.657336</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>44</v>
+      </c>
+      <c r="E19" t="n">
+        <v>80</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>10:33:41</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1765856021.72098</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>71</v>
+      </c>
+      <c r="E20" t="n">
+        <v>93.09999999999999</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10:33:48</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1765856028.505733</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Arrhythmia!</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>136</v>
+      </c>
+      <c r="E21" t="n">
+        <v>97.7</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>10:34:11</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1765856051.126576</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>83</v>
+      </c>
+      <c r="E22" t="n">
+        <v>95.7</v>
+      </c>
+      <c r="F22" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:34:16</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1765856056.40432</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>78</v>
+      </c>
+      <c r="E23" t="n">
+        <v>95.90000000000001</v>
+      </c>
+      <c r="F23" t="n">
+        <v>78</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>10:34:21</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1765856061.687434</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>75</v>
+      </c>
+      <c r="E24" t="n">
+        <v>96.3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:34:26</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1765856066.974875</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>68</v>
+      </c>
+      <c r="E25" t="n">
+        <v>96.09999999999999</v>
+      </c>
+      <c r="F25" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:34:32</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1765856072.26853</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>71</v>
+      </c>
+      <c r="E26" t="n">
+        <v>96.09999999999999</v>
+      </c>
+      <c r="F26" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10:34:37</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1765856077.55586</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>75</v>
+      </c>
+      <c r="E27" t="n">
+        <v>95.90000000000001</v>
+      </c>
+      <c r="F27" t="n">
+        <v>31</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>10:34:42</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1765856082.846297</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>68</v>
+      </c>
+      <c r="E28" t="n">
+        <v>96.40000000000001</v>
+      </c>
+      <c r="F28" t="n">
+        <v>80</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>10:34:48</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1765856088.138705</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>71</v>
+      </c>
+      <c r="E29" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="F29" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>10:35:00</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1765856100.206277</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Arrhythmia!</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>88</v>
+      </c>
+      <c r="E30" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>10:35:05</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1765856105.488332</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>88</v>
+      </c>
+      <c r="E31" t="n">
+        <v>95.7</v>
+      </c>
+      <c r="F31" t="n">
+        <v>31</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>10:35:16</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1765856116.156705</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Stress/Risk</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>100</v>
+      </c>
+      <c r="E32" t="n">
+        <v>94.3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>10:35:21</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1765856121.439722</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>78</v>
+      </c>
+      <c r="E33" t="n">
+        <v>98</v>
+      </c>
+      <c r="F33" t="n">
+        <v>78</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>10:35:26</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1765856126.728537</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>93</v>
+      </c>
+      <c r="E34" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="F34" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10:35:32</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1765856132.018156</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>78</v>
+      </c>
+      <c r="E35" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="F35" t="n">
+        <v>40</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10:35:42</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1765856142.595431</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>75</v>
+      </c>
+      <c r="E36" t="n">
+        <v>96.7</v>
+      </c>
+      <c r="F36" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>10:35:47</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1765856147.882835</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>78</v>
+      </c>
+      <c r="E37" t="n">
+        <v>96</v>
+      </c>
+      <c r="F37" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>10:35:53</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1765856153.169861</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>83</v>
+      </c>
+      <c r="E38" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="F38" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>10:36:13</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1765856173.520646</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>107</v>
+      </c>
+      <c r="E39" t="n">
+        <v>80</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>11:04:24</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>136</v>
+      </c>
+      <c r="E40" t="n">
+        <v>80</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>11:04:47</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>3</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>136</v>
+      </c>
+      <c r="E41" t="n">
+        <v>80</v>
+      </c>
+      <c r="F41" t="n">
+        <v>40</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>11:04:59</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>136</v>
+      </c>
+      <c r="E42" t="n">
+        <v>80</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>11:05:16</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>115</v>
+      </c>
+      <c r="E43" t="n">
+        <v>90.40000000000001</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>11:05:30</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>136</v>
+      </c>
+      <c r="E44" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>11:05:52</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>136</v>
+      </c>
+      <c r="E45" t="n">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>11:23:56</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>136</v>
+      </c>
+      <c r="D46" t="n">
+        <v>83.09999999999999</v>
+      </c>
+      <c r="E46" t="n">
+        <v>40</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>11:25:13</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>136</v>
+      </c>
+      <c r="D47" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>11:25:40</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>71</v>
+      </c>
+      <c r="D48" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="E48" t="n">
+        <v>138.6</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>11:25:52</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>78</v>
+      </c>
+      <c r="D49" t="n">
+        <v>96.40000000000001</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Arrhythmia!</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>11:25:57</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>68</v>
+      </c>
+      <c r="D50" t="n">
+        <v>98</v>
+      </c>
+      <c r="E50" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>11:26:02</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>68</v>
+      </c>
+      <c r="D51" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="E51" t="n">
+        <v>89.40000000000001</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>11:26:14</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>75</v>
+      </c>
+      <c r="D52" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>11:26:32</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>83</v>
+      </c>
+      <c r="D53" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="E53" t="n">
+        <v>103.9</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>11:26:54</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>42</v>
+      </c>
+      <c r="D54" t="n">
+        <v>92.90000000000001</v>
+      </c>
+      <c r="E54" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>11:52:22</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>68</v>
+      </c>
+      <c r="D55" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>11:52:28</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>62</v>
+      </c>
+      <c r="D56" t="n">
+        <v>97.2</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Arrhythmia!</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>11:53:30</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>71</v>
+      </c>
+      <c r="D57" t="n">
+        <v>80</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Low SpO2!</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>